<commit_message>
Update BROObject - GMW IMBRO datafile NL (v1.x).xlsx
</commit_message>
<xml_diff>
--- a/GMW/BROObject - GMW IMBRO datafile NL (v1.x).xlsx
+++ b/GMW/BROObject - GMW IMBRO datafile NL (v1.x).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://3hydro-my.sharepoint.com/personal/jos_von_asmuth_3hydro_nl/Documents/GitHub/BRO-Spreadsheet-en-tabelformat/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trefo\OneDrive - Trefoil Hydrology\GitHub\BRO-Spreadsheet-en-tabelformat\GMW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{B2B2B6C2-F56B-4149-8FD3-56B22F0FB87D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{83946D85-C950-4FE2-A392-EF95845BEDAC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1ED2DD1-39A5-4646-9597-FFCAD7CA7286}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{26814B37-6F38-4D5A-99CF-A0A5CD7480CB}"/>
   </bookViews>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="194">
   <si>
     <t>Format Name</t>
   </si>
@@ -661,6 +661,9 @@
   </si>
   <si>
     <t>elektrodepositie</t>
+  </si>
+  <si>
+    <t>buismateriaal</t>
   </si>
 </sst>
 </file>
@@ -1469,8 +1472,8 @@
   </sheetPr>
   <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1820,12 +1823,6 @@
           </x14:formula1>
           <xm:sqref>L11</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{60DBC67C-2722-4BF1-BCBD-0CAD0E672119}">
-          <x14:formula1>
-            <xm:f>Waardelijsten!$E$2:$E$12</xm:f>
-          </x14:formula1>
-          <xm:sqref>N11</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{57C6B4E6-5591-4EFA-8527-82EB5E59428F}">
           <x14:formula1>
             <xm:f>Waardelijsten!$F$2:$F$3</xm:f>
@@ -1837,6 +1834,12 @@
             <xm:f>Waardelijsten!$G$2:$G$13</xm:f>
           </x14:formula1>
           <xm:sqref>S11</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{60DBC67C-2722-4BF1-BCBD-0CAD0E672119}">
+          <x14:formula1>
+            <xm:f>Waardelijsten!$E$2:$E$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>N11</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1851,8 +1854,8 @@
   </sheetPr>
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="14.4"/>
@@ -1913,7 +1916,7 @@
         <v>176</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>175</v>
+        <v>193</v>
       </c>
       <c r="M1" s="9" t="s">
         <v>177</v>
@@ -2297,7 +2300,7 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2538,7 +2541,7 @@
         <v>58</v>
       </c>
       <c r="E5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G5" t="s">
         <v>76</v>
@@ -2573,7 +2576,7 @@
         <v>59</v>
       </c>
       <c r="E6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G6" t="s">
         <v>77</v>
@@ -2599,7 +2602,7 @@
         <v>47</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G7" t="s">
         <v>78</v>

</xml_diff>